<commit_message>
Adding use case and scenario
</commit_message>
<xml_diff>
--- a/documentation/useCase-scenario/scenarios.xlsx
+++ b/documentation/useCase-scenario/scenarios.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projet-WEB\LoCar\useCase-scenario\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projet-WEB\LoCar\documentation\useCase-scenario\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="découvrir" sheetId="1" r:id="rId1"/>
@@ -17,8 +17,10 @@
     <sheet name="détails" sheetId="3" r:id="rId3"/>
     <sheet name="s'enregistrer" sheetId="5" r:id="rId4"/>
     <sheet name="loger" sheetId="4" r:id="rId5"/>
-    <sheet name="Feuil2" sheetId="7" r:id="rId6"/>
+    <sheet name="créer une offre" sheetId="7" r:id="rId6"/>
     <sheet name="modifier" sheetId="6" r:id="rId7"/>
+    <sheet name="suppression" sheetId="8" r:id="rId8"/>
+    <sheet name="filtres" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="95">
   <si>
     <t>En tant que</t>
   </si>
@@ -258,6 +260,63 @@
   </si>
   <si>
     <t>Mettre à disposition ma voiture</t>
+  </si>
+  <si>
+    <t>Je me logue</t>
+  </si>
+  <si>
+    <t>(faire le scénario LC005)</t>
+  </si>
+  <si>
+    <t>La nouvelle page d'accueil apparaît:</t>
+  </si>
+  <si>
+    <t>Je clique sur créer une offre</t>
+  </si>
+  <si>
+    <t>La page de création d'offre apparaît:</t>
+  </si>
+  <si>
+    <t>Création d'offre</t>
+  </si>
+  <si>
+    <t>Pour valider je clique sur: " créer"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> La page de toutes les offres s'affiche</t>
+  </si>
+  <si>
+    <t>LC008 - Supprimer une offre</t>
+  </si>
+  <si>
+    <t>Supprimer l'une de mes offres</t>
+  </si>
+  <si>
+    <t>L'enlever du site</t>
+  </si>
+  <si>
+    <t>Je clique sur: "supprimer" de l'offre que je veux modifier</t>
+  </si>
+  <si>
+    <t>Suppression</t>
+  </si>
+  <si>
+    <t>LC009 - Filtre</t>
+  </si>
+  <si>
+    <t>Filtrer les offres</t>
+  </si>
+  <si>
+    <t>La confirmation de la supression apparaît:</t>
+  </si>
+  <si>
+    <t>Les voire dans un autre ordre</t>
+  </si>
+  <si>
+    <t>Dans le filtre de gauche je tape Yverdon-les-bain et dans celui de droite les prix décroissants</t>
+  </si>
+  <si>
+    <t>Seul les annonces qui sont localisées à yverdon s'affichent et dans l'orde des prix décroissants:</t>
   </si>
 </sst>
 </file>
@@ -527,7 +586,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -598,6 +657,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1012,7 +1074,7 @@
   <dimension ref="B1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E11" sqref="B11:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1503,7 +1565,7 @@
   <dimension ref="B1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1645,10 +1707,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F18"/>
+  <dimension ref="B1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1733,45 +1795,53 @@
       </c>
       <c r="F10" s="12"/>
     </row>
-    <row r="11" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="20" t="s">
-        <v>51</v>
+        <v>76</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="E11" s="24" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F11" s="12"/>
     </row>
-    <row r="12" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="C12" s="21" t="s">
-        <v>53</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="C12" s="21"/>
       <c r="D12" s="22" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="E12" s="24" t="s">
-        <v>54</v>
+        <v>81</v>
       </c>
       <c r="F12" s="12"/>
     </row>
-    <row r="13" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="16"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="19"/>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="C13" s="21"/>
+      <c r="D13" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="E13" s="24" t="s">
+        <v>31</v>
+      </c>
       <c r="F13" s="12"/>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="11"/>
+    <row r="14" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="16"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="12"/>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="11"/>
@@ -1782,11 +1852,15 @@
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" s="11"/>
     </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="11"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E11" r:id="rId1"/>
-    <hyperlink ref="E10" r:id="rId2"/>
+    <hyperlink ref="E10" r:id="rId1"/>
+    <hyperlink ref="E11" r:id="rId2"/>
     <hyperlink ref="E12" r:id="rId3"/>
+    <hyperlink ref="E13" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1939,4 +2013,295 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:F18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.140625" customWidth="1"/>
+    <col min="2" max="3" width="32.5703125" customWidth="1"/>
+    <col min="4" max="4" width="34.140625" customWidth="1"/>
+    <col min="5" max="5" width="32.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="13"/>
+    </row>
+    <row r="3" spans="2:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="13"/>
+    </row>
+    <row r="4" spans="2:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="D4" s="13"/>
+    </row>
+    <row r="5" spans="2:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="D5" s="13"/>
+    </row>
+    <row r="6" spans="2:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="13"/>
+    </row>
+    <row r="8" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="15"/>
+      <c r="D10" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" s="12"/>
+    </row>
+    <row r="11" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B11" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="E11" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="F11" s="12"/>
+    </row>
+    <row r="12" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B12" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="E12" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="F12" s="12"/>
+    </row>
+    <row r="13" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="16"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="12"/>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="11"/>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="11"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="11"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="11"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E11" r:id="rId1"/>
+    <hyperlink ref="E10" r:id="rId2"/>
+    <hyperlink ref="E12" r:id="rId3"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:F18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="B9:E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.140625" customWidth="1"/>
+    <col min="2" max="3" width="32.5703125" customWidth="1"/>
+    <col min="4" max="4" width="34.140625" customWidth="1"/>
+    <col min="5" max="5" width="32.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" s="13"/>
+    </row>
+    <row r="3" spans="2:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="13"/>
+    </row>
+    <row r="4" spans="2:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D4" s="13"/>
+    </row>
+    <row r="5" spans="2:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="D5" s="13"/>
+    </row>
+    <row r="6" spans="2:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="13"/>
+    </row>
+    <row r="8" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="15"/>
+      <c r="D10" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" s="12"/>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="21"/>
+      <c r="D11" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="12"/>
+    </row>
+    <row r="12" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B12" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="C12" s="21"/>
+      <c r="D12" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="E12" s="24"/>
+      <c r="F12" s="12"/>
+    </row>
+    <row r="13" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="16"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="12"/>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="11"/>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="11"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="11"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="11"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E10" r:id="rId1"/>
+    <hyperlink ref="E11" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>